<commit_message>
updated, removed old directory
</commit_message>
<xml_diff>
--- a/Bill of Materials/BOM.xlsx
+++ b/Bill of Materials/BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
   <si>
     <t>Core2 X48 Motherboard Bill of Materials</t>
   </si>
@@ -124,6 +124,12 @@
   </si>
   <si>
     <t>Intel Core2 CPU</t>
+  </si>
+  <si>
+    <t>Gigabit LAN Chip</t>
+  </si>
+  <si>
+    <t>Gigabit Platform LAN Connect</t>
   </si>
 </sst>
 </file>
@@ -210,12 +216,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -224,6 +227,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -519,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:M15"/>
+  <dimension ref="B3:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -542,20 +551,20 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:13" ht="21.75" thickBot="1">
-      <c r="C3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+      <c r="C3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
     </row>
     <row r="4" spans="2:13" ht="15.75" thickBot="1">
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="3">
         <v>4</v>
       </c>
     </row>
@@ -765,7 +774,7 @@
       <c r="F12" t="s">
         <v>28</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="4">
         <v>475053305</v>
       </c>
       <c r="K12">
@@ -850,6 +859,23 @@
       <c r="M15">
         <f t="shared" si="2"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13">
+      <c r="C16">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" s="5">
+        <v>82566</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added all initial items from big picture diagram
</commit_message>
<xml_diff>
--- a/Bill of Materials/BOM.xlsx
+++ b/Bill of Materials/BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>Core2 X48 Motherboard Bill of Materials</t>
   </si>
@@ -130,6 +130,30 @@
   </si>
   <si>
     <t>Gigabit Platform LAN Connect</t>
+  </si>
+  <si>
+    <t>Gigabit Socket</t>
+  </si>
+  <si>
+    <t>USB Connector</t>
+  </si>
+  <si>
+    <t>BIOS EEPROM</t>
+  </si>
+  <si>
+    <t>Winbond</t>
+  </si>
+  <si>
+    <t>16Mbit W25X16BV EEPROM</t>
+  </si>
+  <si>
+    <t>W25X16BVDAI</t>
+  </si>
+  <si>
+    <t>SATA Data Connector</t>
+  </si>
+  <si>
+    <t>Connector for Signals of SATA drive</t>
   </si>
 </sst>
 </file>
@@ -528,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:M16"/>
+  <dimension ref="B3:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -631,7 +655,7 @@
     </row>
     <row r="8" spans="2:13">
       <c r="B8">
-        <f t="shared" ref="B8:B15" si="0">IF(E8="",0,IF(F8="",1,IF(H8="",2,3)))</f>
+        <f t="shared" ref="B8:B20" si="0">IF(E8="",0,IF(F8="",1,IF(H8="",2,3)))</f>
         <v>2</v>
       </c>
       <c r="C8">
@@ -862,6 +886,10 @@
       </c>
     </row>
     <row r="16" spans="2:13">
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
       <c r="C16">
         <v>10</v>
       </c>
@@ -876,19 +904,140 @@
       </c>
       <c r="G16" s="5">
         <v>82566</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <f t="shared" ref="L16:L19" si="3">K16*$K$4</f>
+        <v>4</v>
+      </c>
+      <c r="M16">
+        <f t="shared" ref="M16:M19" si="4">L16*J16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13">
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>11</v>
+      </c>
+      <c r="D17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" s="5">
+        <v>471554001</v>
+      </c>
+      <c r="K17">
+        <v>5</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13">
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>13</v>
+      </c>
+      <c r="D18" t="s">
+        <v>38</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13">
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>14</v>
+      </c>
+      <c r="D19" t="s">
+        <v>39</v>
+      </c>
+      <c r="K19">
+        <v>12</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13">
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>15</v>
+      </c>
+      <c r="D20" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20" t="s">
+        <v>43</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <f t="shared" ref="L20" si="5">K20*$K$4</f>
+        <v>4</v>
+      </c>
+      <c r="M20">
+        <f t="shared" ref="M20" si="6">L20*J20</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C3:H3"/>
   </mergeCells>
-  <conditionalFormatting sqref="A7:B7 B8:B15">
+  <conditionalFormatting sqref="A7:B7 B8:B20">
     <cfRule type="expression" priority="2">
       <formula>"if($E$7="""";true;false)"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7:B15">
-    <cfRule type="iconSet" priority="1">
+  <conditionalFormatting sqref="B7:B20">
+    <cfRule type="iconSet" priority="6">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>

</xml_diff>

<commit_message>
updated BOM with most part info
</commit_message>
<xml_diff>
--- a/Bill of Materials/BOM.xlsx
+++ b/Bill of Materials/BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="81">
   <si>
     <t>Core2 X48 Motherboard Bill of Materials</t>
   </si>
@@ -144,23 +144,131 @@
     <t>Winbond</t>
   </si>
   <si>
-    <t>16Mbit W25X16BV EEPROM</t>
-  </si>
-  <si>
-    <t>W25X16BVDAI</t>
-  </si>
-  <si>
     <t>SATA Data Connector</t>
   </si>
   <si>
     <t>Connector for Signals of SATA drive</t>
+  </si>
+  <si>
+    <t>Web Link</t>
+  </si>
+  <si>
+    <t>http://www.silego.com/store/product_info.php?cPath=24_30&amp;products_id=150</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Must order qty 10 @ $5.00 ea for total of $50.00</t>
+  </si>
+  <si>
+    <t>SLG505YC256BT</t>
+  </si>
+  <si>
+    <t>http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=WM7359-ND</t>
+  </si>
+  <si>
+    <t>WM7359-ND</t>
+  </si>
+  <si>
+    <t>Digikey</t>
+  </si>
+  <si>
+    <t>http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=WM9003-ND</t>
+  </si>
+  <si>
+    <t>WM9003-ND</t>
+  </si>
+  <si>
+    <t>http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=WM19104-ND</t>
+  </si>
+  <si>
+    <t>WM19104-ND</t>
+  </si>
+  <si>
+    <t>67800-5005</t>
+  </si>
+  <si>
+    <t>W25Q16BVSSIG-ND</t>
+  </si>
+  <si>
+    <t>W25Q16BV</t>
+  </si>
+  <si>
+    <t>16Mbit W25Q16BV EEPROM</t>
+  </si>
+  <si>
+    <t>http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=W25Q16BVSSIG-ND</t>
+  </si>
+  <si>
+    <t>Other Charges</t>
+  </si>
+  <si>
+    <t>Connector for 10/100/1000 network</t>
+  </si>
+  <si>
+    <t>Dual port stack USB 2.0 through hole connecotr</t>
+  </si>
+  <si>
+    <t>Tyco</t>
+  </si>
+  <si>
+    <t>5787745-2-ND</t>
+  </si>
+  <si>
+    <t>5787745-1</t>
+  </si>
+  <si>
+    <t>http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=5787745-2-ND</t>
+  </si>
+  <si>
+    <t>507-1425-ND</t>
+  </si>
+  <si>
+    <t>http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=507-1425-ND</t>
+  </si>
+  <si>
+    <t>0826-1A1T-23-F</t>
+  </si>
+  <si>
+    <t>Bel Fuse</t>
+  </si>
+  <si>
+    <t>RU82566DM S L95J</t>
+  </si>
+  <si>
+    <t>Arrow</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>16 week lead time</t>
+  </si>
+  <si>
+    <t>http://www.newegg.com/Product/Product.aspx?Item=N82E16819115056</t>
+  </si>
+  <si>
+    <t>NewEgg</t>
+  </si>
+  <si>
+    <t>N82E16819115056</t>
+  </si>
+  <si>
+    <t>E7500</t>
+  </si>
+  <si>
+    <t>Core2 Duo 2.93GHz 3MB L2 65W</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,6 +300,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -237,10 +352,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -255,11 +374,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -552,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:M20"/>
+  <dimension ref="B3:P35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -568,31 +690,34 @@
     <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9" customWidth="1"/>
+    <col min="15" max="15" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="43.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:13" ht="21.75" thickBot="1">
-      <c r="C3" s="6" t="s">
+    <row r="3" spans="2:16" ht="21.75" thickBot="1">
+      <c r="C3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-    </row>
-    <row r="4" spans="2:13" ht="15.75" thickBot="1">
-      <c r="J4" s="2" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+    </row>
+    <row r="4" spans="2:16" ht="15.75" thickBot="1">
+      <c r="K4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="3">
+      <c r="L4" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:13">
+    <row r="6" spans="2:16">
       <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
@@ -615,19 +740,28 @@
         <v>7</v>
       </c>
       <c r="J6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="N6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="O6" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="2:13">
+      <c r="P6" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16">
       <c r="B7">
         <f>IF(E7="",0,IF(F7="",1,IF(H7="",2,3)))</f>
         <v>1</v>
@@ -641,19 +775,21 @@
       <c r="E7" t="s">
         <v>11</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="7"/>
+      <c r="L7">
         <v>1</v>
       </c>
-      <c r="L7">
-        <f>K7*$K$4</f>
+      <c r="M7">
+        <f>L7*$L$4</f>
         <v>4</v>
       </c>
-      <c r="M7">
-        <f>L7*J7</f>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7">
+        <f>M7*K7+N7</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:13">
+    <row r="8" spans="2:16">
       <c r="B8">
         <f t="shared" ref="B8:B20" si="0">IF(E8="",0,IF(F8="",1,IF(H8="",2,3)))</f>
         <v>2</v>
@@ -673,19 +809,21 @@
       <c r="G8" t="s">
         <v>18</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="7"/>
+      <c r="L8">
         <v>1</v>
       </c>
-      <c r="L8">
-        <f t="shared" ref="L8:L15" si="1">K8*$K$4</f>
+      <c r="M8">
+        <f t="shared" ref="M8:M15" si="1">L8*$L$4</f>
         <v>4</v>
       </c>
-      <c r="M8">
-        <f t="shared" ref="M8:M15" si="2">L8*J8</f>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7">
+        <f t="shared" ref="O8:O20" si="2">M8*K8+N8</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:13">
+    <row r="9" spans="2:16">
       <c r="B9">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -705,22 +843,24 @@
       <c r="G9" t="s">
         <v>21</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="7"/>
+      <c r="L9">
         <v>1</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="M9">
+      <c r="N9" s="7"/>
+      <c r="O9" s="7">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:13">
+    <row r="10" spans="2:16">
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C10">
         <v>4</v>
@@ -737,109 +877,154 @@
       <c r="G10" t="s">
         <v>24</v>
       </c>
-      <c r="K10">
+      <c r="H10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" t="s">
+        <v>48</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="K10" s="7">
+        <v>5</v>
+      </c>
+      <c r="L10">
         <v>1</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="M10">
+      <c r="N10" s="7">
+        <v>30</v>
+      </c>
+      <c r="O10" s="7">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="P10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16">
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" t="s">
+        <v>51</v>
+      </c>
+      <c r="I11" t="s">
+        <v>50</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K11" s="7">
+        <v>5.09</v>
+      </c>
+      <c r="L11">
+        <v>4</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7">
+        <f t="shared" si="2"/>
+        <v>81.44</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16">
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="4">
+        <v>475053305</v>
+      </c>
+      <c r="H12" t="s">
+        <v>51</v>
+      </c>
+      <c r="I12" t="s">
+        <v>53</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="K12" s="7">
+        <v>5.03</v>
+      </c>
+      <c r="L12">
+        <v>2</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7">
+        <f t="shared" si="2"/>
+        <v>40.24</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16">
+      <c r="B13">
+        <f>IF(E13="",0,IF(F13="",1,IF(H17="",2,3)))</f>
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" t="s">
+        <v>33</v>
+      </c>
+      <c r="L13">
+        <v>4</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:13">
-      <c r="B11">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="C11">
-        <v>5</v>
-      </c>
-      <c r="D11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" t="s">
-        <v>28</v>
-      </c>
-      <c r="G11" t="s">
-        <v>29</v>
-      </c>
-      <c r="K11">
-        <v>4</v>
-      </c>
-      <c r="L11">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="M11">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:13">
-      <c r="B12">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="C12">
-        <v>6</v>
-      </c>
-      <c r="D12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" t="s">
-        <v>28</v>
-      </c>
-      <c r="G12" s="4">
-        <v>475053305</v>
-      </c>
-      <c r="K12">
-        <v>2</v>
-      </c>
-      <c r="L12">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="M12">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:13">
-      <c r="B13">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>7</v>
-      </c>
-      <c r="D13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" t="s">
-        <v>33</v>
-      </c>
-      <c r="K13">
-        <v>4</v>
-      </c>
-      <c r="L13">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="M13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:13">
+    <row r="14" spans="2:16">
       <c r="B14">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -850,22 +1035,24 @@
       <c r="D14" t="s">
         <v>34</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="7"/>
+      <c r="L14">
         <v>1</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="M14">
+      <c r="N14" s="7"/>
+      <c r="O14" s="7">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:13">
+    <row r="15" spans="2:16">
       <c r="B15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C15">
         <v>9</v>
@@ -873,22 +1060,44 @@
       <c r="D15" t="s">
         <v>35</v>
       </c>
-      <c r="K15">
+      <c r="E15" t="s">
+        <v>80</v>
+      </c>
+      <c r="F15" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" t="s">
+        <v>79</v>
+      </c>
+      <c r="H15" t="s">
+        <v>77</v>
+      </c>
+      <c r="I15" t="s">
+        <v>78</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="K15" s="7">
+        <v>124.99</v>
+      </c>
+      <c r="L15">
         <v>1</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="M15">
+      <c r="N15" s="7"/>
+      <c r="O15" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:13">
+        <v>499.96</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16">
       <c r="B16">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C16">
         <v>10</v>
@@ -905,54 +1114,83 @@
       <c r="G16" s="5">
         <v>82566</v>
       </c>
-      <c r="K16">
+      <c r="H16" t="s">
+        <v>73</v>
+      </c>
+      <c r="I16" t="s">
+        <v>72</v>
+      </c>
+      <c r="J16" t="s">
+        <v>74</v>
+      </c>
+      <c r="K16" s="7">
+        <v>6.69</v>
+      </c>
+      <c r="L16">
         <v>1</v>
       </c>
-      <c r="L16">
-        <f t="shared" ref="L16:L19" si="3">K16*$K$4</f>
+      <c r="M16">
+        <f t="shared" ref="M16:M19" si="3">L16*$L$4</f>
         <v>4</v>
       </c>
-      <c r="M16">
-        <f t="shared" ref="M16:M19" si="4">L16*J16</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13">
+      <c r="N16" s="7"/>
+      <c r="O16" s="7">
+        <f t="shared" si="2"/>
+        <v>26.76</v>
+      </c>
+      <c r="P16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15">
       <c r="B17">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C17">
         <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F17" t="s">
         <v>28</v>
       </c>
-      <c r="G17" s="5">
-        <v>471554001</v>
-      </c>
-      <c r="K17">
+      <c r="G17" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H17" t="s">
+        <v>51</v>
+      </c>
+      <c r="I17" t="s">
+        <v>55</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="K17" s="7">
+        <v>1.012</v>
+      </c>
+      <c r="L17">
         <v>5</v>
       </c>
-      <c r="L17">
+      <c r="M17">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="M17">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:13">
+      <c r="N17" s="7"/>
+      <c r="O17" s="7">
+        <f t="shared" si="2"/>
+        <v>20.240000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15">
       <c r="B18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C18">
         <v>13</v>
@@ -960,22 +1198,44 @@
       <c r="D18" t="s">
         <v>38</v>
       </c>
-      <c r="K18">
+      <c r="E18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18" t="s">
+        <v>71</v>
+      </c>
+      <c r="G18" t="s">
+        <v>70</v>
+      </c>
+      <c r="H18" t="s">
+        <v>51</v>
+      </c>
+      <c r="I18" t="s">
+        <v>68</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="K18" s="7">
+        <v>4.92</v>
+      </c>
+      <c r="L18">
         <v>1</v>
       </c>
-      <c r="L18">
+      <c r="M18">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="M18">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13">
+      <c r="N18" s="7"/>
+      <c r="O18" s="7">
+        <f t="shared" si="2"/>
+        <v>19.68</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15">
       <c r="B19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C19">
         <v>14</v>
@@ -983,22 +1243,44 @@
       <c r="D19" t="s">
         <v>39</v>
       </c>
-      <c r="K19">
-        <v>12</v>
+      <c r="E19" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" t="s">
+        <v>64</v>
+      </c>
+      <c r="G19" t="s">
+        <v>66</v>
+      </c>
+      <c r="H19" t="s">
+        <v>51</v>
+      </c>
+      <c r="I19" t="s">
+        <v>65</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="K19" s="7">
+        <v>2.4500000000000002</v>
       </c>
       <c r="L19">
+        <v>6</v>
+      </c>
+      <c r="M19">
         <f t="shared" si="3"/>
-        <v>48</v>
-      </c>
-      <c r="M19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:13">
+        <v>24</v>
+      </c>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7">
+        <f t="shared" si="2"/>
+        <v>58.800000000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15">
       <c r="B20">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C20">
         <v>15</v>
@@ -1007,24 +1289,43 @@
         <v>40</v>
       </c>
       <c r="E20" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="F20" t="s">
         <v>41</v>
       </c>
       <c r="G20" t="s">
-        <v>43</v>
-      </c>
-      <c r="K20">
+        <v>58</v>
+      </c>
+      <c r="H20" t="s">
+        <v>51</v>
+      </c>
+      <c r="I20" t="s">
+        <v>57</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="K20" s="7">
+        <v>3.27</v>
+      </c>
+      <c r="L20">
         <v>1</v>
       </c>
-      <c r="L20">
-        <f t="shared" ref="L20" si="5">K20*$K$4</f>
+      <c r="M20">
+        <f t="shared" ref="M20" si="4">L20*$L$4</f>
         <v>4</v>
       </c>
-      <c r="M20">
-        <f t="shared" ref="M20" si="6">L20*J20</f>
-        <v>0</v>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7">
+        <f t="shared" si="2"/>
+        <v>13.08</v>
+      </c>
+    </row>
+    <row r="35" spans="15:15">
+      <c r="O35" s="7">
+        <f>SUM(O7:O34)</f>
+        <v>810.19999999999993</v>
       </c>
     </row>
   </sheetData>
@@ -1046,8 +1347,18 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="J10" r:id="rId1"/>
+    <hyperlink ref="J11" r:id="rId2"/>
+    <hyperlink ref="J12" r:id="rId3"/>
+    <hyperlink ref="J17" r:id="rId4"/>
+    <hyperlink ref="J20" r:id="rId5"/>
+    <hyperlink ref="J19" r:id="rId6"/>
+    <hyperlink ref="J18" r:id="rId7"/>
+    <hyperlink ref="J15" r:id="rId8"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added demo price for intel parts not available online added datasheet for gig-E connector
</commit_message>
<xml_diff>
--- a/Bill of Materials/BOM.xlsx
+++ b/Bill of Materials/BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="91">
   <si>
     <t>Core2 X48 Motherboard Bill of Materials</t>
   </si>
@@ -117,9 +117,6 @@
     <t>DDR3 800 1GB Module</t>
   </si>
   <si>
-    <t>Main memory</t>
-  </si>
-  <si>
     <t>Video Card</t>
   </si>
   <si>
@@ -259,6 +256,39 @@
   </si>
   <si>
     <t>Core2 Duo 2.93GHz 3MB L2 65W</t>
+  </si>
+  <si>
+    <t>http://www.newegg.com/Product/Product.aspx?Item=N82E16820148147</t>
+  </si>
+  <si>
+    <t>N82E1682014814</t>
+  </si>
+  <si>
+    <t>CT12864BA1067</t>
+  </si>
+  <si>
+    <t>Crucial</t>
+  </si>
+  <si>
+    <t>1GB DDR3 1066MHz SDRAM</t>
+  </si>
+  <si>
+    <t>http://www.newegg.com/Product/Product.aspx?Item=N82E16814127473</t>
+  </si>
+  <si>
+    <t>N82E16814127473</t>
+  </si>
+  <si>
+    <t>N8400GS-D256H</t>
+  </si>
+  <si>
+    <t>MSI</t>
+  </si>
+  <si>
+    <t>GeForce 8400 GS 256MB 64-bit DDR2 PCI Express 2.0 x16</t>
+  </si>
+  <si>
+    <t>*</t>
   </si>
 </sst>
 </file>
@@ -359,7 +389,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -379,6 +409,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -674,10 +705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:P35"/>
+  <dimension ref="A3:P35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -695,11 +726,11 @@
     <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9" customWidth="1"/>
-    <col min="15" max="15" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="43.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:16" ht="21.75" thickBot="1">
+    <row r="3" spans="1:16" ht="21.75" thickBot="1">
       <c r="C3" s="8" t="s">
         <v>0</v>
       </c>
@@ -709,7 +740,7 @@
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
     </row>
-    <row r="4" spans="2:16" ht="15.75" thickBot="1">
+    <row r="4" spans="1:16" ht="15.75" thickBot="1">
       <c r="K4" s="2" t="s">
         <v>14</v>
       </c>
@@ -717,7 +748,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:16">
+    <row r="6" spans="1:16">
       <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
@@ -740,7 +771,7 @@
         <v>7</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>8</v>
@@ -752,17 +783,20 @@
         <v>13</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16">
-      <c r="B7">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B7" s="9">
         <f>IF(E7="",0,IF(F7="",1,IF(H7="",2,3)))</f>
         <v>1</v>
       </c>
@@ -775,7 +809,9 @@
       <c r="E7" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="7"/>
+      <c r="K7" s="7">
+        <v>30</v>
+      </c>
       <c r="L7">
         <v>1</v>
       </c>
@@ -786,11 +822,14 @@
       <c r="N7" s="7"/>
       <c r="O7" s="7">
         <f>M7*K7+N7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:16">
-      <c r="B8">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" s="9">
         <f t="shared" ref="B8:B20" si="0">IF(E8="",0,IF(F8="",1,IF(H8="",2,3)))</f>
         <v>2</v>
       </c>
@@ -809,7 +848,9 @@
       <c r="G8" t="s">
         <v>18</v>
       </c>
-      <c r="K8" s="7"/>
+      <c r="K8" s="7">
+        <v>50</v>
+      </c>
       <c r="L8">
         <v>1</v>
       </c>
@@ -820,11 +861,14 @@
       <c r="N8" s="7"/>
       <c r="O8" s="7">
         <f t="shared" ref="O8:O20" si="2">M8*K8+N8</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:16">
-      <c r="B9">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" s="9">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -843,7 +887,9 @@
       <c r="G9" t="s">
         <v>21</v>
       </c>
-      <c r="K9" s="7"/>
+      <c r="K9" s="7">
+        <v>30</v>
+      </c>
       <c r="L9">
         <v>1</v>
       </c>
@@ -854,11 +900,11 @@
       <c r="N9" s="7"/>
       <c r="O9" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:16">
-      <c r="B10">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="B10" s="9">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -881,10 +927,10 @@
         <v>23</v>
       </c>
       <c r="I10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K10" s="7">
         <v>5</v>
@@ -904,11 +950,11 @@
         <v>50</v>
       </c>
       <c r="P10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="2:16">
-      <c r="B11">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="B11" s="9">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -928,13 +974,13 @@
         <v>29</v>
       </c>
       <c r="H11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K11" s="7">
         <v>5.09</v>
@@ -952,8 +998,8 @@
         <v>81.44</v>
       </c>
     </row>
-    <row r="12" spans="2:16">
-      <c r="B12">
+    <row r="12" spans="1:16">
+      <c r="B12" s="9">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -973,13 +1019,13 @@
         <v>475053305</v>
       </c>
       <c r="H12" t="s">
+        <v>50</v>
+      </c>
+      <c r="I12" t="s">
+        <v>52</v>
+      </c>
+      <c r="J12" s="6" t="s">
         <v>51</v>
-      </c>
-      <c r="I12" t="s">
-        <v>53</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>52</v>
       </c>
       <c r="K12" s="7">
         <v>5.03</v>
@@ -997,10 +1043,10 @@
         <v>40.24</v>
       </c>
     </row>
-    <row r="13" spans="2:16">
-      <c r="B13">
-        <f>IF(E13="",0,IF(F13="",1,IF(H17="",2,3)))</f>
-        <v>1</v>
+    <row r="13" spans="1:16">
+      <c r="B13" s="9">
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="C13">
         <v>7</v>
@@ -1009,7 +1055,25 @@
         <v>32</v>
       </c>
       <c r="E13" t="s">
-        <v>33</v>
+        <v>84</v>
+      </c>
+      <c r="F13" t="s">
+        <v>83</v>
+      </c>
+      <c r="G13" t="s">
+        <v>82</v>
+      </c>
+      <c r="H13" t="s">
+        <v>76</v>
+      </c>
+      <c r="I13" t="s">
+        <v>81</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="K13" s="7">
+        <v>23.99</v>
       </c>
       <c r="L13">
         <v>4</v>
@@ -1021,21 +1085,41 @@
       <c r="N13" s="7"/>
       <c r="O13" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:16">
-      <c r="B14">
+        <v>383.84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="B14" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C14">
         <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
-      </c>
-      <c r="K14" s="7"/>
+        <v>33</v>
+      </c>
+      <c r="E14" t="s">
+        <v>89</v>
+      </c>
+      <c r="F14" t="s">
+        <v>88</v>
+      </c>
+      <c r="G14" t="s">
+        <v>87</v>
+      </c>
+      <c r="H14" t="s">
+        <v>76</v>
+      </c>
+      <c r="I14" t="s">
+        <v>86</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="K14" s="7">
+        <v>27</v>
+      </c>
       <c r="L14">
         <v>1</v>
       </c>
@@ -1046,11 +1130,14 @@
       <c r="N14" s="7"/>
       <c r="O14" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:16">
-      <c r="B15">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" s="9">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -1058,25 +1145,25 @@
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F15" t="s">
         <v>17</v>
       </c>
       <c r="G15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H15" t="s">
+        <v>76</v>
+      </c>
+      <c r="I15" t="s">
         <v>77</v>
       </c>
-      <c r="I15" t="s">
-        <v>78</v>
-      </c>
       <c r="J15" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K15" s="7">
         <v>124.99</v>
@@ -1094,8 +1181,11 @@
         <v>499.96</v>
       </c>
     </row>
-    <row r="16" spans="2:16">
-      <c r="B16">
+    <row r="16" spans="1:16">
+      <c r="A16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B16" s="9">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -1103,10 +1193,10 @@
         <v>10</v>
       </c>
       <c r="D16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" t="s">
         <v>36</v>
-      </c>
-      <c r="E16" t="s">
-        <v>37</v>
       </c>
       <c r="F16" t="s">
         <v>17</v>
@@ -1115,13 +1205,13 @@
         <v>82566</v>
       </c>
       <c r="H16" t="s">
+        <v>72</v>
+      </c>
+      <c r="I16" t="s">
+        <v>71</v>
+      </c>
+      <c r="J16" t="s">
         <v>73</v>
-      </c>
-      <c r="I16" t="s">
-        <v>72</v>
-      </c>
-      <c r="J16" t="s">
-        <v>74</v>
       </c>
       <c r="K16" s="7">
         <v>6.69</v>
@@ -1139,11 +1229,11 @@
         <v>26.76</v>
       </c>
       <c r="P16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="2:15">
-      <c r="B17">
+      <c r="B17" s="9">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -1151,25 +1241,25 @@
         <v>11</v>
       </c>
       <c r="D17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" t="s">
         <v>42</v>
-      </c>
-      <c r="E17" t="s">
-        <v>43</v>
       </c>
       <c r="F17" t="s">
         <v>28</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K17" s="7">
         <v>1.012</v>
@@ -1188,7 +1278,7 @@
       </c>
     </row>
     <row r="18" spans="2:15">
-      <c r="B18">
+      <c r="B18" s="9">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -1196,25 +1286,25 @@
         <v>13</v>
       </c>
       <c r="D18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I18" t="s">
+        <v>67</v>
+      </c>
+      <c r="J18" s="6" t="s">
         <v>68</v>
-      </c>
-      <c r="J18" s="6" t="s">
-        <v>69</v>
       </c>
       <c r="K18" s="7">
         <v>4.92</v>
@@ -1233,7 +1323,7 @@
       </c>
     </row>
     <row r="19" spans="2:15">
-      <c r="B19">
+      <c r="B19" s="9">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -1241,25 +1331,25 @@
         <v>14</v>
       </c>
       <c r="D19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E19" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" t="s">
         <v>63</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
+        <v>65</v>
+      </c>
+      <c r="H19" t="s">
+        <v>50</v>
+      </c>
+      <c r="I19" t="s">
         <v>64</v>
       </c>
-      <c r="G19" t="s">
+      <c r="J19" s="6" t="s">
         <v>66</v>
-      </c>
-      <c r="H19" t="s">
-        <v>51</v>
-      </c>
-      <c r="I19" t="s">
-        <v>65</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>67</v>
       </c>
       <c r="K19" s="7">
         <v>2.4500000000000002</v>
@@ -1278,7 +1368,7 @@
       </c>
     </row>
     <row r="20" spans="2:15">
-      <c r="B20">
+      <c r="B20" s="9">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -1286,25 +1376,25 @@
         <v>15</v>
       </c>
       <c r="D20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" t="s">
         <v>40</v>
       </c>
-      <c r="E20" t="s">
+      <c r="G20" t="s">
+        <v>57</v>
+      </c>
+      <c r="H20" t="s">
+        <v>50</v>
+      </c>
+      <c r="I20" t="s">
+        <v>56</v>
+      </c>
+      <c r="J20" s="6" t="s">
         <v>59</v>
-      </c>
-      <c r="F20" t="s">
-        <v>41</v>
-      </c>
-      <c r="G20" t="s">
-        <v>58</v>
-      </c>
-      <c r="H20" t="s">
-        <v>51</v>
-      </c>
-      <c r="I20" t="s">
-        <v>57</v>
-      </c>
-      <c r="J20" s="6" t="s">
-        <v>60</v>
       </c>
       <c r="K20" s="7">
         <v>3.27</v>
@@ -1325,7 +1415,7 @@
     <row r="35" spans="15:15">
       <c r="O35" s="7">
         <f>SUM(O7:O34)</f>
-        <v>810.19999999999993</v>
+        <v>1742.04</v>
       </c>
     </row>
   </sheetData>
@@ -1356,9 +1446,11 @@
     <hyperlink ref="J19" r:id="rId6"/>
     <hyperlink ref="J18" r:id="rId7"/>
     <hyperlink ref="J15" r:id="rId8"/>
+    <hyperlink ref="J13" r:id="rId9"/>
+    <hyperlink ref="J14" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added misc. items (HD,on-board connectors for power)
</commit_message>
<xml_diff>
--- a/Bill of Materials/BOM.xlsx
+++ b/Bill of Materials/BOM.xlsx
@@ -11,12 +11,15 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="CART_ITEM" localSheetId="0">Sheet1!$G$22</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="108">
   <si>
     <t>Core2 X48 Motherboard Bill of Materials</t>
   </si>
@@ -307,6 +310,39 @@
   </si>
   <si>
     <t>http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=631-1015-1-ND</t>
+  </si>
+  <si>
+    <t>Hard Drive</t>
+  </si>
+  <si>
+    <t>250GB SATAII</t>
+  </si>
+  <si>
+    <t>Hitachi</t>
+  </si>
+  <si>
+    <t>HTS545025B9A300</t>
+  </si>
+  <si>
+    <t>N82E16822145255</t>
+  </si>
+  <si>
+    <t>http://www.newegg.com/Product/Product.aspx?Item=N82E16822145255</t>
+  </si>
+  <si>
+    <t>Discount ends 8/25</t>
+  </si>
+  <si>
+    <t>CPU Fan</t>
+  </si>
+  <si>
+    <t>24 pin Power Connector</t>
+  </si>
+  <si>
+    <t>12v Power Connector</t>
+  </si>
+  <si>
+    <t>Fan Connectors</t>
   </si>
 </sst>
 </file>
@@ -725,8 +761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:P35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="G4" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -848,7 +884,7 @@
         <v>90</v>
       </c>
       <c r="B8" s="8">
-        <f t="shared" ref="B8:B21" si="0">IF(E8="",0,IF(F8="",1,IF(H8="",2,3)))</f>
+        <f t="shared" ref="B8:B26" si="0">IF(E8="",0,IF(F8="",1,IF(H8="",2,3)))</f>
         <v>2</v>
       </c>
       <c r="C8">
@@ -878,7 +914,7 @@
       </c>
       <c r="N8" s="7"/>
       <c r="O8" s="7">
-        <f t="shared" ref="O8:O21" si="2">M8*K8+N8</f>
+        <f t="shared" ref="O8:O22" si="2">M8*K8+N8</f>
         <v>200</v>
       </c>
     </row>
@@ -1250,7 +1286,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="2:15">
+    <row r="17" spans="2:16">
       <c r="B17" s="8">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1295,7 +1331,7 @@
         <v>20.240000000000002</v>
       </c>
     </row>
-    <row r="18" spans="2:15">
+    <row r="18" spans="2:16">
       <c r="B18" s="8">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1340,7 +1376,7 @@
         <v>19.68</v>
       </c>
     </row>
-    <row r="19" spans="2:15">
+    <row r="19" spans="2:16">
       <c r="B19" s="8">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1385,7 +1421,7 @@
         <v>58.800000000000004</v>
       </c>
     </row>
-    <row r="20" spans="2:15">
+    <row r="20" spans="2:16">
       <c r="B20" s="8">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1421,7 +1457,7 @@
         <v>1</v>
       </c>
       <c r="M20">
-        <f t="shared" ref="M20:M21" si="4">L20*$L$4</f>
+        <f t="shared" ref="M20:M22" si="4">L20*$L$4</f>
         <v>4</v>
       </c>
       <c r="N20" s="7"/>
@@ -1430,7 +1466,7 @@
         <v>13.08</v>
       </c>
     </row>
-    <row r="21" spans="2:15">
+    <row r="21" spans="2:16">
       <c r="B21" s="8">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1474,22 +1510,165 @@
         <v>2.48</v>
       </c>
     </row>
+    <row r="22" spans="2:16">
+      <c r="B22" s="8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>17</v>
+      </c>
+      <c r="D22" t="s">
+        <v>97</v>
+      </c>
+      <c r="E22" t="s">
+        <v>98</v>
+      </c>
+      <c r="F22" t="s">
+        <v>99</v>
+      </c>
+      <c r="G22" t="s">
+        <v>100</v>
+      </c>
+      <c r="H22" t="s">
+        <v>76</v>
+      </c>
+      <c r="I22" t="s">
+        <v>101</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="K22" s="7">
+        <v>34.99</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="O22" s="7">
+        <f t="shared" si="2"/>
+        <v>139.96</v>
+      </c>
+      <c r="P22" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16">
+      <c r="B23" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>18</v>
+      </c>
+      <c r="D23" t="s">
+        <v>104</v>
+      </c>
+      <c r="K23" s="7"/>
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="M23">
+        <f t="shared" ref="M23:M26" si="5">L23*$L$4</f>
+        <v>4</v>
+      </c>
+      <c r="O23" s="7">
+        <f t="shared" ref="O23:O26" si="6">M23*K23+N23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16">
+      <c r="B24" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>19</v>
+      </c>
+      <c r="D24" t="s">
+        <v>105</v>
+      </c>
+      <c r="K24" s="7"/>
+      <c r="L24">
+        <v>1</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="O24" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16">
+      <c r="B25" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>20</v>
+      </c>
+      <c r="D25" t="s">
+        <v>106</v>
+      </c>
+      <c r="K25" s="7"/>
+      <c r="L25">
+        <v>1</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="O25" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16">
+      <c r="B26" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>21</v>
+      </c>
+      <c r="D26" t="s">
+        <v>107</v>
+      </c>
+      <c r="K26" s="7"/>
+      <c r="L26">
+        <v>1</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="O26" s="7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
     <row r="35" spans="15:15">
       <c r="O35" s="7">
         <f>SUM(O7:O34)</f>
-        <v>1744.52</v>
+        <v>1884.48</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C3:H3"/>
   </mergeCells>
-  <conditionalFormatting sqref="A7:B7 B8:B21">
+  <conditionalFormatting sqref="A7:B7 B8:B26">
     <cfRule type="expression" priority="2">
       <formula>"if($E$7="""";true;false)"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7:B21">
+  <conditionalFormatting sqref="B7:B26">
     <cfRule type="iconSet" priority="6">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
@@ -1511,9 +1690,10 @@
     <hyperlink ref="J13" r:id="rId9"/>
     <hyperlink ref="J14" r:id="rId10"/>
     <hyperlink ref="J21" r:id="rId11"/>
+    <hyperlink ref="J22" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
fan connectors, bios chip socket
</commit_message>
<xml_diff>
--- a/Bill of Materials/BOM.xlsx
+++ b/Bill of Materials/BOM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="135" windowWidth="21720" windowHeight="9780"/>
@@ -15,12 +15,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$6:$P$6</definedName>
     <definedName name="CART_ITEM" localSheetId="0">Sheet1!$G$22</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="137">
   <si>
     <t>Core2 X48 Motherboard Bill of Materials</t>
   </si>
@@ -401,6 +401,36 @@
   </si>
   <si>
     <t>CONN HEADER 4POS 4.2MM VERT TIN</t>
+  </si>
+  <si>
+    <t>http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=WM4202-ND</t>
+  </si>
+  <si>
+    <t>WM4202-ND</t>
+  </si>
+  <si>
+    <t>22-23-2041</t>
+  </si>
+  <si>
+    <t>CONN HEADER 4POS .100 VERT TIN</t>
+  </si>
+  <si>
+    <t>http://search.digikey.com/scripts/DkSearch/dksus.dll?Detail&amp;name=3M5461-ND</t>
+  </si>
+  <si>
+    <t>3M5461-ND</t>
+  </si>
+  <si>
+    <t>4808-3000-CP</t>
+  </si>
+  <si>
+    <t>3M</t>
+  </si>
+  <si>
+    <t>SOCKET IC OPEN FRAME 8POS .3"</t>
+  </si>
+  <si>
+    <t>BIOS Socket</t>
   </si>
 </sst>
 </file>
@@ -862,7 +892,7 @@
   <dimension ref="A2:P35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -967,7 +997,7 @@
         <v>90</v>
       </c>
       <c r="B7" s="22">
-        <f t="shared" ref="B7:B27" si="0">IF(E7="",0,IF(F7="",1,IF(H7="",2,3)))</f>
+        <f t="shared" ref="B7:B28" si="0">IF(E7="",0,IF(F7="",1,IF(H7="",2,3)))</f>
         <v>3</v>
       </c>
       <c r="C7" s="21">
@@ -1001,12 +1031,12 @@
         <v>1</v>
       </c>
       <c r="M7" s="21">
-        <f t="shared" ref="M7:M27" si="1">L7*$L$4</f>
+        <f t="shared" ref="M7:M28" si="1">L7*$L$4</f>
         <v>4</v>
       </c>
       <c r="N7" s="24"/>
       <c r="O7" s="24">
-        <f t="shared" ref="O7:O27" si="2">M7*K7+N7</f>
+        <f t="shared" ref="O7:O28" si="2">M7*K7+N7</f>
         <v>26.76</v>
       </c>
       <c r="P7" s="21" t="s">
@@ -1808,7 +1838,7 @@
     <row r="26" spans="1:16">
       <c r="B26" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C26">
         <v>21</v>
@@ -1816,17 +1846,37 @@
       <c r="D26" t="s">
         <v>107</v>
       </c>
-      <c r="K26" s="5"/>
+      <c r="E26" t="s">
+        <v>130</v>
+      </c>
+      <c r="F26" t="s">
+        <v>28</v>
+      </c>
+      <c r="G26" t="s">
+        <v>129</v>
+      </c>
+      <c r="H26" t="s">
+        <v>50</v>
+      </c>
+      <c r="I26" t="s">
+        <v>128</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="K26" s="5">
+        <v>0.41499999999999998</v>
+      </c>
       <c r="L26">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M26">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="O26" s="5">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.64</v>
       </c>
     </row>
     <row r="27" spans="1:16">
@@ -1873,10 +1923,54 @@
         <v>67.959999999999994</v>
       </c>
     </row>
+    <row r="28" spans="1:16">
+      <c r="B28" s="6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <v>23</v>
+      </c>
+      <c r="D28" t="s">
+        <v>136</v>
+      </c>
+      <c r="E28" t="s">
+        <v>135</v>
+      </c>
+      <c r="F28" t="s">
+        <v>134</v>
+      </c>
+      <c r="G28" t="s">
+        <v>133</v>
+      </c>
+      <c r="H28" t="s">
+        <v>50</v>
+      </c>
+      <c r="I28" t="s">
+        <v>132</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="K28" s="5">
+        <v>0.21</v>
+      </c>
+      <c r="L28">
+        <v>1</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="O28" s="5">
+        <f t="shared" si="2"/>
+        <v>0.84</v>
+      </c>
+    </row>
     <row r="35" spans="15:15">
       <c r="O35" s="5">
         <f>SUM(O7:O34)</f>
-        <v>2010.0400000000002</v>
+        <v>2017.5200000000002</v>
       </c>
     </row>
   </sheetData>
@@ -1889,12 +1983,27 @@
     <mergeCell ref="C3:H3"/>
   </mergeCells>
   <conditionalFormatting sqref="A7:B7 B8:B27">
+    <cfRule type="expression" priority="4">
+      <formula>"if($E$7="""";true;false)"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:B27">
+    <cfRule type="iconSet" priority="8">
+      <iconSet iconSet="4TrafficLights">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="2"/>
+        <cfvo type="num" val="3"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B28">
     <cfRule type="expression" priority="2">
       <formula>"if($E$7="""";true;false)"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7:B27">
-    <cfRule type="iconSet" priority="6">
+  <conditionalFormatting sqref="B28">
+    <cfRule type="iconSet" priority="1">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -1920,9 +2029,11 @@
     <hyperlink ref="J27" r:id="rId14"/>
     <hyperlink ref="J24" r:id="rId15"/>
     <hyperlink ref="J25" r:id="rId16"/>
+    <hyperlink ref="J26" r:id="rId17"/>
+    <hyperlink ref="J28" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
 

</xml_diff>